<commit_message>
Added Mapping column to import excel
</commit_message>
<xml_diff>
--- a/CrossFinance/DetailFormatInExcel/aTest.xlsx
+++ b/CrossFinance/DetailFormatInExcel/aTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21630" windowHeight="5055"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,9 @@
     <t>SecondName</t>
   </si>
   <si>
-    <t>Surname</t>
-  </si>
-  <si>
-    <t>NationalIdentificationNumber</t>
-  </si>
-  <si>
     <t>AddressId</t>
   </si>
   <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>PhoneNumber2</t>
-  </si>
-  <si>
     <t>Marcin</t>
   </si>
   <si>
@@ -48,7 +36,19 @@
     <t>Rak1</t>
   </si>
   <si>
-    <t>Imię</t>
+    <t>imie</t>
+  </si>
+  <si>
+    <t>nazwisko</t>
+  </si>
+  <si>
+    <t>PESEL</t>
+  </si>
+  <si>
+    <t>Telefon 1</t>
+  </si>
+  <si>
+    <t>Telefon2</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -405,33 +407,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>676767676</v>
@@ -448,10 +450,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>676767676</v>

</xml_diff>

<commit_message>
Added data.cs and Exel method
</commit_message>
<xml_diff>
--- a/CrossFinance/DetailFormatInExcel/aTest.xlsx
+++ b/CrossFinance/DetailFormatInExcel/aTest.xlsx
@@ -16,25 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>SecondName</t>
-  </si>
-  <si>
-    <t>AddressId</t>
-  </si>
-  <si>
-    <t>Marcin</t>
-  </si>
-  <si>
-    <t>Rak</t>
-  </si>
-  <si>
-    <t>Marcin1</t>
-  </si>
-  <si>
-    <t>Rak1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>imie</t>
   </si>
@@ -49,13 +31,127 @@
   </si>
   <si>
     <t>Telefon2</t>
+  </si>
+  <si>
+    <t>lp</t>
+  </si>
+  <si>
+    <t>nr_umowy</t>
+  </si>
+  <si>
+    <t>MAIN_STREET_NAME</t>
+  </si>
+  <si>
+    <t>MAIN_STREET_NUMBER</t>
+  </si>
+  <si>
+    <t>MAIN_STREET_FLAT_NUMBER</t>
+  </si>
+  <si>
+    <t>MAIN_POST_CODE</t>
+  </si>
+  <si>
+    <t>MAIN_POST_OFFICE_CITY</t>
+  </si>
+  <si>
+    <t>CORRESPONDENCE_STREET_NAME</t>
+  </si>
+  <si>
+    <t>CORRESPONDENCE_STREET_NUMBER</t>
+  </si>
+  <si>
+    <t>CORRESPONDENCE_STREET_FLAT_NUMBER</t>
+  </si>
+  <si>
+    <t>CORRESPONDENCE_POST_CODE</t>
+  </si>
+  <si>
+    <t>CORRESPONDENCE_POST_OFFICE_CITY</t>
+  </si>
+  <si>
+    <t>Kapital</t>
+  </si>
+  <si>
+    <t>odsetki</t>
+  </si>
+  <si>
+    <t>odsetki Karne</t>
+  </si>
+  <si>
+    <t>opłaty</t>
+  </si>
+  <si>
+    <t>koszty sadowe</t>
+  </si>
+  <si>
+    <t>koszty zastepstwa sadowego</t>
+  </si>
+  <si>
+    <t>koszty egzekucji</t>
+  </si>
+  <si>
+    <t>koszty zastepstwa egzekucyjnego</t>
+  </si>
+  <si>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>KRZYSZTOF</t>
+  </si>
+  <si>
+    <t>KUFEL</t>
+  </si>
+  <si>
+    <t>Objazdowa</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>58-506</t>
+  </si>
+  <si>
+    <t>Jelenia Góra</t>
+  </si>
+  <si>
+    <t>Poetów</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1234567810</t>
+  </si>
+  <si>
+    <t>SEBASTIAN</t>
+  </si>
+  <si>
+    <t>KULAK</t>
+  </si>
+  <si>
+    <t>Stefana Batorego</t>
+  </si>
+  <si>
+    <t>5/7</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>58-500</t>
+  </si>
+  <si>
+    <t>Krasińskiego</t>
+  </si>
+  <si>
+    <t>20D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +159,20 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -73,7 +183,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,12 +191,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -388,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,68 +540,222 @@
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="1">
+        <v>81052439121</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="1">
+        <v>45</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="1">
+        <v>125652158</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>125652177</v>
+      </c>
+      <c r="R2" s="1">
+        <v>13.12</v>
+      </c>
+      <c r="S2" s="1">
+        <v>1703</v>
+      </c>
+      <c r="T2" s="1">
+        <v>15</v>
+      </c>
+      <c r="U2" s="1">
+        <v>30</v>
+      </c>
+      <c r="V2" s="1">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1">
+        <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>12345</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>676767676</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1234511</v>
-      </c>
-      <c r="B3">
-        <v>1234511</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>676767676</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
+      <c r="B3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="1">
+        <v>86090717811</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="1">
+        <v>11</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1">
+        <v>125652159</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>125652178</v>
+      </c>
+      <c r="R3" s="1">
+        <v>1138.0999999999999</v>
+      </c>
+      <c r="S3" s="1">
+        <v>647</v>
+      </c>
+      <c r="T3" s="1">
+        <v>45</v>
+      </c>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>